<commit_message>
remove outliers in exposure to coas t
</commit_message>
<xml_diff>
--- a/results/categories.xlsx
+++ b/results/categories.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="73">
   <si>
     <t>resilience</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Ilocos Sur</t>
   </si>
   <si>
-    <t>Iloilo</t>
-  </si>
-  <si>
     <t>Isabela</t>
   </si>
   <si>
@@ -214,16 +211,10 @@
     <t>Sultan Kudarat</t>
   </si>
   <si>
-    <t>Sulu</t>
-  </si>
-  <si>
     <t>Surigao Del Norte</t>
   </si>
   <si>
     <t>Tarlac</t>
-  </si>
-  <si>
-    <t>Tawi-Tawi</t>
   </si>
   <si>
     <t>Zambales</t>
@@ -618,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -647,10 +638,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -658,10 +649,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -669,10 +660,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -680,10 +671,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -691,10 +682,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -702,10 +693,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -713,10 +704,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -724,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -735,10 +726,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -746,10 +737,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -757,10 +748,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -768,10 +759,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -779,10 +770,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -790,10 +781,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -801,10 +792,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -812,10 +803,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -823,10 +814,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -834,10 +825,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -845,10 +836,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -856,10 +847,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -867,10 +858,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -878,10 +869,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -889,10 +880,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -900,10 +891,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -911,10 +902,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -922,10 +913,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -933,10 +924,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -944,10 +935,10 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -955,10 +946,10 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -966,10 +957,10 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -977,10 +968,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -988,10 +979,10 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -999,10 +990,10 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1010,10 +1001,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1021,10 +1012,10 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1032,10 +1023,10 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1043,10 +1034,10 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1054,10 +1045,10 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1065,10 +1056,10 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1076,10 +1067,10 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1087,10 +1078,10 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1098,10 +1089,10 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1109,10 +1100,10 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1120,10 +1111,10 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1131,10 +1122,10 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1142,10 +1133,10 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1153,10 +1144,10 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1164,10 +1155,10 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1175,10 +1166,10 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1186,10 +1177,10 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1197,10 +1188,10 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1208,10 +1199,10 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1219,10 +1210,10 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1230,10 +1221,10 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1241,10 +1232,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1252,10 +1243,10 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1263,10 +1254,10 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1274,10 +1265,10 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1285,10 +1276,10 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1296,10 +1287,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1307,10 +1298,10 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1318,10 +1309,10 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1329,10 +1320,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1340,10 +1331,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1351,10 +1342,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1362,10 +1353,10 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1373,10 +1364,10 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1384,43 +1375,10 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" t="s">
-        <v>74</v>
-      </c>
-      <c r="C72" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
putting back the possibility of multi_hazard_data, and populates hazard data with coastal flood data for illustration purposes
</commit_message>
<xml_diff>
--- a/results/categories.xlsx
+++ b/results/categories.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="67">
   <si>
     <t>risk_to_assets</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Abra</t>
   </si>
   <si>
-    <t>Agusan Del Norte</t>
-  </si>
-  <si>
-    <t>Agusan Del Sur</t>
-  </si>
-  <si>
     <t>Aklan</t>
   </si>
   <si>
@@ -58,6 +52,9 @@
     <t>Bataan</t>
   </si>
   <si>
+    <t>Batanes</t>
+  </si>
+  <si>
     <t>Batangas</t>
   </si>
   <si>
@@ -100,12 +97,6 @@
     <t>Compostela Valley</t>
   </si>
   <si>
-    <t>Davao Del Norte</t>
-  </si>
-  <si>
-    <t>Davao Del Sur</t>
-  </si>
-  <si>
     <t>Davao Oriental</t>
   </si>
   <si>
@@ -136,12 +127,6 @@
     <t>Laguna</t>
   </si>
   <si>
-    <t>Lanao Del Norte</t>
-  </si>
-  <si>
-    <t>Lanao Del Sur</t>
-  </si>
-  <si>
     <t>Leyte</t>
   </si>
   <si>
@@ -154,13 +139,16 @@
     <t>Masbate</t>
   </si>
   <si>
+    <t>Misamis Occidental</t>
+  </si>
+  <si>
     <t>Misamis Oriental</t>
   </si>
   <si>
     <t>Negros Occidental</t>
   </si>
   <si>
-    <t>North Cotabato</t>
+    <t>Negros Oriental</t>
   </si>
   <si>
     <t>Northern Samar</t>
@@ -196,12 +184,12 @@
     <t>Romblon</t>
   </si>
   <si>
-    <t>Samar</t>
-  </si>
-  <si>
     <t>Sarangani</t>
   </si>
   <si>
+    <t>Siquijor</t>
+  </si>
+  <si>
     <t>Sorsogon</t>
   </si>
   <si>
@@ -214,31 +202,22 @@
     <t>Sultan Kudarat</t>
   </si>
   <si>
-    <t>Surigao Del Norte</t>
-  </si>
-  <si>
     <t>Tarlac</t>
   </si>
   <si>
     <t>Zambales</t>
   </si>
   <si>
-    <t>Zamboanga Del Norte</t>
-  </si>
-  <si>
-    <t>Zamboanga Del Sur</t>
-  </si>
-  <si>
     <t>Zamboanga Sibugay</t>
   </si>
   <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>Mid</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -612,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -644,13 +623,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -658,13 +637,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -672,13 +651,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -686,13 +665,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -700,13 +679,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -714,13 +693,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -728,13 +707,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -742,13 +721,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -756,13 +735,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -770,13 +749,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -784,13 +763,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -798,13 +777,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -812,13 +791,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -826,13 +805,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -840,13 +819,13 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -854,13 +833,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -868,13 +847,13 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -882,13 +861,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -896,13 +875,13 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -910,13 +889,13 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -924,13 +903,13 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -938,13 +917,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -952,13 +931,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -966,13 +945,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -980,13 +959,13 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -994,13 +973,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1008,13 +987,13 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1022,13 +1001,13 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1036,13 +1015,13 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1050,13 +1029,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1064,13 +1043,13 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1078,13 +1057,13 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1092,13 +1071,13 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1106,13 +1085,13 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1120,13 +1099,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1134,13 +1113,13 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1148,13 +1127,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1162,13 +1141,13 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1176,13 +1155,13 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1190,13 +1169,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1204,13 +1183,13 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1218,13 +1197,13 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1232,13 +1211,13 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1246,13 +1225,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1260,13 +1239,13 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D46" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1274,13 +1253,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1288,13 +1267,13 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D48" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1302,13 +1281,13 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1316,13 +1295,13 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D50" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1330,13 +1309,13 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1344,13 +1323,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D52" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1358,13 +1337,13 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1372,13 +1351,13 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1386,13 +1365,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1400,13 +1379,13 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1414,13 +1393,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1428,13 +1407,13 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1442,13 +1421,13 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1456,13 +1435,13 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1470,13 +1449,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1484,111 +1463,13 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D64" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" t="s">
-        <v>72</v>
-      </c>
-      <c r="D65" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" t="s">
-        <v>72</v>
-      </c>
-      <c r="D66" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" t="s">
-        <v>71</v>
-      </c>
-      <c r="C67" t="s">
-        <v>73</v>
-      </c>
-      <c r="D67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68" t="s">
-        <v>71</v>
-      </c>
-      <c r="D68" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" t="s">
-        <v>73</v>
-      </c>
-      <c r="C69" t="s">
-        <v>73</v>
-      </c>
-      <c r="D69" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model and data as to march 17th
</commit_message>
<xml_diff>
--- a/results/categories.xlsx
+++ b/results/categories.xlsx
@@ -211,13 +211,13 @@
     <t>Zamboanga Sibugay</t>
   </si>
   <si>
+    <t>Mid</t>
+  </si>
+  <si>
     <t>High</t>
   </si>
   <si>
     <t>Low</t>
-  </si>
-  <si>
-    <t>Mid</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -637,13 +637,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -651,13 +651,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -665,13 +665,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -679,13 +679,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -693,13 +693,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -707,13 +707,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -721,13 +721,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -735,13 +735,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -749,13 +749,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -763,13 +763,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -777,13 +777,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -791,10 +791,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>66</v>
@@ -805,13 +805,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -822,7 +822,7 @@
         <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>64</v>
@@ -833,13 +833,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -850,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
         <v>64</v>
@@ -864,10 +864,10 @@
         <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -878,7 +878,7 @@
         <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
@@ -889,13 +889,13 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -903,13 +903,13 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -917,13 +917,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -931,13 +931,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -945,13 +945,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -959,13 +959,13 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -973,13 +973,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -990,7 +990,7 @@
         <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
         <v>66</v>
@@ -1004,10 +1004,10 @@
         <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1018,10 +1018,10 @@
         <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1032,10 +1032,10 @@
         <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1046,10 +1046,10 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1057,13 +1057,13 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1071,13 +1071,13 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1085,13 +1085,13 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1099,13 +1099,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1113,13 +1113,13 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1127,13 +1127,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1141,10 +1141,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
         <v>64</v>
@@ -1155,13 +1155,13 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1169,10 +1169,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D41" t="s">
         <v>64</v>
@@ -1183,10 +1183,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>66</v>
@@ -1197,13 +1197,13 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1214,7 +1214,7 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D44" t="s">
         <v>64</v>
@@ -1228,7 +1228,7 @@
         <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
         <v>64</v>
@@ -1242,10 +1242,10 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1253,13 +1253,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1267,13 +1267,13 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1284,7 +1284,7 @@
         <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
         <v>66</v>
@@ -1295,10 +1295,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
         <v>64</v>
@@ -1312,7 +1312,7 @@
         <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D51" t="s">
         <v>66</v>
@@ -1323,13 +1323,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1337,13 +1337,13 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1351,10 +1351,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D54" t="s">
         <v>66</v>
@@ -1365,13 +1365,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1379,13 +1379,13 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1393,13 +1393,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1407,13 +1407,13 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1424,10 +1424,10 @@
         <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D59" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1438,7 +1438,7 @@
         <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
         <v>66</v>
@@ -1449,13 +1449,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1463,13 +1463,13 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>